<commit_message>
build register xlsx to json
</commit_message>
<xml_diff>
--- a/data/xlsx/Baernreither_Ortsregister_2023.xlsx
+++ b/data/xlsx/Baernreither_Ortsregister_2023.xlsx
@@ -1,26 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christofaichner/Desktop/Kommission f gesch ö/Kommission Aichner/Projekte/Baernreither/Clariah 2022/Register/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13800"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="13800"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
-    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725" refMode="R1C1" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="330"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -37,9 +27,6 @@
     <t>Wien</t>
   </si>
   <si>
-    <t>GeoNames</t>
-  </si>
-  <si>
     <t>Prag</t>
   </si>
   <si>
@@ -712,9 +699,6 @@
     <t>https://d-nb.info/gnd/4280197-7</t>
   </si>
   <si>
-    <t>Keywert</t>
-  </si>
-  <si>
     <t>BadIschl</t>
   </si>
   <si>
@@ -797,6 +781,12 @@
   </si>
   <si>
     <t>https://www.geonames.org/2763587/tyrol.html</t>
+  </si>
+  <si>
+    <t>PID</t>
+  </si>
+  <si>
+    <t>key</t>
   </si>
 </sst>
 </file>
@@ -892,7 +882,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -969,8 +959,8 @@
   <tableColumns count="4">
     <tableColumn id="5" name="Name" dataDxfId="3"/>
     <tableColumn id="1" name="heute" dataDxfId="2"/>
-    <tableColumn id="2" name="GeoNames" dataDxfId="1"/>
-    <tableColumn id="3" name="Keywert" dataDxfId="0"/>
+    <tableColumn id="2" name="PID" dataDxfId="1"/>
+    <tableColumn id="3" name="key" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1265,1196 +1255,1196 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="134" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" style="4" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="74.33203125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="74.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>254</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>227</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>111</v>
-      </c>
       <c r="D7" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>117</v>
-      </c>
       <c r="D12" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>69</v>
-      </c>
       <c r="C18" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>127</v>
-      </c>
       <c r="D23" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="1" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
-        <v>197</v>
-      </c>
       <c r="B35" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="36" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B42" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B43" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="B43" s="4" t="s">
+      <c r="C43" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>82</v>
-      </c>
       <c r="C44" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B45" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="C45" s="5" t="s">
-        <v>223</v>
-      </c>
       <c r="D45" s="4" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B46" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B47" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>85</v>
-      </c>
       <c r="C47" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B49" s="4"/>
       <c r="C49" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B50" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="B51" s="4"/>
       <c r="C51" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B52" s="4"/>
       <c r="C52" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B53" s="4"/>
       <c r="C53" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B54" s="4"/>
       <c r="C54" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B56" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C55" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>89</v>
-      </c>
       <c r="C56" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B57" s="4"/>
       <c r="C57" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B58" s="4"/>
       <c r="C58" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B59" s="4"/>
       <c r="C59" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B60" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B62" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C60" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B62" s="4" t="s">
+      <c r="C62" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B64" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C62" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="D63" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>92</v>
-      </c>
       <c r="C64" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B67" s="4"/>
       <c r="C67" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B68" s="4"/>
       <c r="C68" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B69" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="C69" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
         <v>190</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="4" t="s">
-        <v>191</v>
       </c>
       <c r="B72" s="4"/>
       <c r="C72" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B73" s="4"/>
       <c r="C73" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B74" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B75" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C74" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="D74" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B75" s="4" t="s">
+      <c r="C75" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B77" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C75" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="D75" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A77" s="4" t="s">
+      <c r="C77" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="B77" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>211</v>
-      </c>
       <c r="D77" s="4" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B78" s="4"/>
       <c r="C78" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B79" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B82" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C79" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="D79" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C80" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="C81" s="4" t="s">
+      <c r="C82" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D81" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>173</v>
-      </c>
       <c r="D82" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C84" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="B84" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>207</v>
-      </c>
       <c r="D84" s="6" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C85" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="B85" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="C85" s="5" t="s">
-        <v>179</v>
-      </c>
       <c r="D85" s="4" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B86" s="4"/>
       <c r="C86" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D86" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B87" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D87" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="7" t="s">
         <v>102</v>
-      </c>
-      <c r="C87" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="D87" s="7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="7" t="s">
-        <v>103</v>
       </c>
       <c r="B88" s="7"/>
       <c r="C88" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D88" s="7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C89" s="12" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2516,28 +2506,4 @@
     <tablePart r:id="rId52"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>